<commit_message>
Add faculty meeting too many students fixed
</commit_message>
<xml_diff>
--- a/Real2020Entry1/fromBot_FacultySchedules_1SheetEach.xlsx
+++ b/Real2020Entry1/fromBot_FacultySchedules_1SheetEach.xlsx
@@ -89,123 +89,126 @@
     <t>Tuesday, Feb. 11 3:45 - 4:15</t>
   </si>
   <si>
+    <t>Narain, Vedang</t>
+  </si>
+  <si>
+    <t>Corrette, John</t>
+  </si>
+  <si>
+    <t>Esquival, Emmanual</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Heid, Leslie</t>
+  </si>
+  <si>
+    <t>Advait, Athreya</t>
+  </si>
+  <si>
+    <t>Ward, Erica</t>
+  </si>
+  <si>
+    <t>Evensen, Claire</t>
+  </si>
+  <si>
+    <t>Xiang, Yankai (Mark)</t>
+  </si>
+  <si>
+    <t>Smith, Sarah</t>
+  </si>
+  <si>
+    <t>Steven Allison</t>
+  </si>
+  <si>
+    <t>Hwang, Ahyeon</t>
+  </si>
+  <si>
+    <t>Kramer, Alexander</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t>Scott Atwood</t>
+  </si>
+  <si>
+    <t>Herath, Samantha</t>
+  </si>
+  <si>
+    <t>Hussein, Amina</t>
+  </si>
+  <si>
+    <t>Degan, Alexandra</t>
+  </si>
+  <si>
+    <t>Bardwell</t>
+  </si>
+  <si>
+    <t>Zhu, Hongman</t>
+  </si>
+  <si>
+    <t>Bruce Blumberg</t>
+  </si>
+  <si>
+    <t>Jan, Tzu-Yi (Ian)</t>
+  </si>
+  <si>
+    <t>Brody</t>
+  </si>
+  <si>
     <t>Xu, Angela</t>
   </si>
   <si>
+    <t>Tim Downing</t>
+  </si>
+  <si>
+    <t>Lee, Beoung</t>
+  </si>
+  <si>
+    <t>Dae Seok Eom</t>
+  </si>
+  <si>
     <t>Wang, Harold</t>
   </si>
   <si>
+    <t>Celia Faiola</t>
+  </si>
+  <si>
+    <t>Steve Frank</t>
+  </si>
+  <si>
     <t>Bartas, Katrina</t>
   </si>
   <si>
-    <t>Xiang, Yankai (Mark)</t>
-  </si>
-  <si>
-    <t>Corrette, John</t>
-  </si>
-  <si>
-    <t>Jan, Tzu-Yi (Ian)</t>
-  </si>
-  <si>
-    <t>Hwang, Ahyeon</t>
-  </si>
-  <si>
-    <t>Heid, Leslie</t>
+    <t>Ermoshkin, Maxim</t>
+  </si>
+  <si>
+    <t>Anya Grosberg</t>
+  </si>
+  <si>
+    <t>Sousa, Rachel</t>
+  </si>
+  <si>
+    <t>Shen, Jiayi</t>
+  </si>
+  <si>
+    <t>Khattab, Sara</t>
+  </si>
+  <si>
+    <t>Wayne Hayes</t>
   </si>
   <si>
     <t>Czarnecki, Paulina</t>
   </si>
   <si>
-    <t>Sousa, Rachel</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>Du, Mingyu</t>
   </si>
   <si>
-    <t>Steven Allison</t>
-  </si>
-  <si>
     <t>Nguyen, Nguyen</t>
   </si>
   <si>
-    <t>Kramer, Alexander</t>
-  </si>
-  <si>
-    <t>Narain, Vedang</t>
-  </si>
-  <si>
-    <t>...</t>
-  </si>
-  <si>
-    <t>Scott Atwood</t>
-  </si>
-  <si>
-    <t>Esquival, Emmanual</t>
-  </si>
-  <si>
-    <t>Khattab, Sara</t>
-  </si>
-  <si>
-    <t>Ermoshkin, Maxim</t>
-  </si>
-  <si>
-    <t>Bardwell</t>
-  </si>
-  <si>
-    <t>Advait, Athreya</t>
-  </si>
-  <si>
-    <t>Ward, Erica</t>
-  </si>
-  <si>
-    <t>Bruce Blumberg</t>
-  </si>
-  <si>
-    <t>Brody</t>
-  </si>
-  <si>
-    <t>Herath, Samantha</t>
-  </si>
-  <si>
-    <t>Tim Downing</t>
-  </si>
-  <si>
-    <t>Lee, Beoung</t>
-  </si>
-  <si>
-    <t>Evensen, Claire</t>
-  </si>
-  <si>
-    <t>Dae Seok Eom</t>
-  </si>
-  <si>
-    <t>Degan, Alexandra</t>
-  </si>
-  <si>
-    <t>Hussein, Amina</t>
-  </si>
-  <si>
-    <t>Zhu, Hongman</t>
-  </si>
-  <si>
-    <t>Celia Faiola</t>
-  </si>
-  <si>
-    <t>Steve Frank</t>
-  </si>
-  <si>
-    <t>Anya Grosberg</t>
-  </si>
-  <si>
-    <t>Wayne Hayes</t>
-  </si>
-  <si>
-    <t>Smith, Sarah</t>
-  </si>
-  <si>
     <t>Lander</t>
   </si>
   <si>
@@ -246,9 +249,6 @@
   </si>
   <si>
     <t>Knut Solna</t>
-  </si>
-  <si>
-    <t>Shen, Jiayi</t>
   </si>
   <si>
     <t>Swarup</t>
@@ -725,7 +725,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -733,7 +733,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -741,7 +741,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -763,7 +763,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -771,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -779,7 +779,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -787,7 +787,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -795,7 +795,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -803,7 +803,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -811,7 +811,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -819,7 +819,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -827,7 +827,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -835,7 +835,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -843,7 +843,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -851,7 +851,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -859,7 +859,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -881,7 +881,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -897,7 +897,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -905,7 +905,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -913,7 +913,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -921,7 +921,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -929,7 +929,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -937,7 +937,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -945,7 +945,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -953,7 +953,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -961,7 +961,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -969,7 +969,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -977,7 +977,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -999,7 +999,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1007,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1015,7 +1015,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1023,7 +1023,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1031,7 +1031,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1039,7 +1039,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1047,7 +1047,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1055,7 +1055,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1063,7 +1063,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1071,7 +1071,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1079,7 +1079,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1087,7 +1087,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1095,7 +1095,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1117,7 +1117,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1125,7 +1125,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1133,7 +1133,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1141,7 +1141,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1149,7 +1149,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1157,7 +1157,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1165,7 +1165,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1173,7 +1173,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1181,7 +1181,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1189,7 +1189,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1197,7 +1197,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1205,7 +1205,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1213,7 +1213,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1235,7 +1235,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1243,7 +1243,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1251,7 +1251,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1259,7 +1259,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1267,7 +1267,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1275,7 +1275,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1283,7 +1283,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1291,7 +1291,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1299,7 +1299,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1307,7 +1307,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1315,7 +1315,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1331,7 +1331,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1353,7 +1353,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1369,7 +1369,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1377,7 +1377,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1385,7 +1385,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1393,7 +1393,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1401,7 +1401,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1409,7 +1409,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1417,7 +1417,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1425,7 +1425,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1433,7 +1433,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1441,7 +1441,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1449,7 +1449,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1471,7 +1471,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1479,7 +1479,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1487,7 +1487,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1495,7 +1495,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1503,7 +1503,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1511,7 +1511,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1519,7 +1519,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1527,7 +1527,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1535,7 +1535,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1543,7 +1543,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1551,7 +1551,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1559,7 +1559,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1567,7 +1567,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1589,7 +1589,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1597,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1605,7 +1605,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1613,7 +1613,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1621,7 +1621,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1629,7 +1629,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1637,7 +1637,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1645,7 +1645,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1653,7 +1653,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1661,7 +1661,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1669,7 +1669,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1677,7 +1677,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1685,7 +1685,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1707,7 +1707,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1715,7 +1715,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1723,7 +1723,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1731,7 +1731,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1739,7 +1739,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1747,7 +1747,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1755,7 +1755,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1763,7 +1763,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1771,7 +1771,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1779,7 +1779,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1787,7 +1787,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1795,7 +1795,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1803,7 +1803,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1825,7 +1825,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1833,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1841,7 +1841,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1849,7 +1849,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1857,7 +1857,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1865,7 +1865,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1873,7 +1873,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1881,7 +1881,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1889,7 +1889,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1897,7 +1897,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1905,7 +1905,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1913,7 +1913,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1921,7 +1921,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1943,7 +1943,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1951,7 +1951,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1959,7 +1959,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1967,7 +1967,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1975,7 +1975,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1983,7 +1983,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1991,7 +1991,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1999,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2007,7 +2007,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2015,7 +2015,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2023,7 +2023,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2031,7 +2031,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2039,7 +2039,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2061,7 +2061,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2069,7 +2069,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2077,7 +2077,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2085,7 +2085,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2093,7 +2093,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2101,7 +2101,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2109,7 +2109,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2117,7 +2117,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2125,7 +2125,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2133,7 +2133,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2141,7 +2141,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2149,7 +2149,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2157,7 +2157,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2179,7 +2179,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2187,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2195,7 +2195,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2203,7 +2203,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2211,7 +2211,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2219,7 +2219,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2227,7 +2227,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2235,7 +2235,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2243,7 +2243,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2251,7 +2251,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2259,7 +2259,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2267,7 +2267,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2275,7 +2275,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2297,7 +2297,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2305,7 +2305,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2313,7 +2313,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2321,7 +2321,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2329,7 +2329,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2337,7 +2337,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2345,7 +2345,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2353,7 +2353,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2361,7 +2361,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2369,7 +2369,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2377,7 +2377,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2385,7 +2385,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2393,7 +2393,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2415,7 +2415,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2423,7 +2423,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2431,7 +2431,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2439,7 +2439,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2447,7 +2447,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2455,7 +2455,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2463,7 +2463,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2471,7 +2471,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2479,7 +2479,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2487,7 +2487,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2495,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2503,7 +2503,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2511,7 +2511,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2533,7 +2533,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2541,7 +2541,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2549,7 +2549,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2565,7 +2565,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2573,7 +2573,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2581,7 +2581,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2589,7 +2589,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2597,7 +2597,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2605,7 +2605,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2613,7 +2613,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2621,7 +2621,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2629,7 +2629,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2651,7 +2651,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2659,7 +2659,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2667,7 +2667,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2675,7 +2675,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2683,7 +2683,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2691,7 +2691,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2699,7 +2699,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2707,7 +2707,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2715,7 +2715,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2723,7 +2723,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2731,7 +2731,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2739,7 +2739,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2747,7 +2747,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2769,7 +2769,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2777,7 +2777,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2785,7 +2785,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2793,7 +2793,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2801,7 +2801,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2809,7 +2809,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2817,7 +2817,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2825,7 +2825,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2833,7 +2833,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2841,7 +2841,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2849,7 +2849,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2857,7 +2857,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2865,7 +2865,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2895,7 +2895,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2903,7 +2903,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2911,7 +2911,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2919,7 +2919,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2927,7 +2927,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2935,7 +2935,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2943,7 +2943,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2951,7 +2951,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2959,7 +2959,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2967,7 +2967,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2975,7 +2975,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2983,7 +2983,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3013,7 +3013,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3021,7 +3021,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3029,7 +3029,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3037,7 +3037,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3045,7 +3045,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3053,7 +3053,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3061,7 +3061,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3069,7 +3069,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3077,7 +3077,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3085,7 +3085,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3093,7 +3093,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3101,7 +3101,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3131,7 +3131,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3139,7 +3139,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3147,7 +3147,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3155,7 +3155,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3163,7 +3163,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3171,7 +3171,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3179,7 +3179,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3187,7 +3187,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3195,7 +3195,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3203,7 +3203,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3211,7 +3211,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3219,7 +3219,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3241,7 +3241,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3249,7 +3249,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3257,7 +3257,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3265,7 +3265,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3273,7 +3273,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3281,7 +3281,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3289,7 +3289,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3297,7 +3297,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3305,7 +3305,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3313,7 +3313,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3321,7 +3321,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3329,7 +3329,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3337,7 +3337,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3367,7 +3367,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3375,7 +3375,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3383,7 +3383,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3391,7 +3391,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3399,7 +3399,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3407,7 +3407,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3415,7 +3415,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3423,7 +3423,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3431,7 +3431,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3439,7 +3439,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3447,7 +3447,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3455,7 +3455,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3485,7 +3485,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3493,7 +3493,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3501,7 +3501,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3509,7 +3509,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3517,7 +3517,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3525,7 +3525,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3533,7 +3533,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3541,7 +3541,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3549,7 +3549,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3557,7 +3557,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3565,7 +3565,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3573,7 +3573,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3603,7 +3603,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3611,7 +3611,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3619,7 +3619,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3627,7 +3627,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3635,7 +3635,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3643,7 +3643,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3651,7 +3651,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3659,7 +3659,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3667,7 +3667,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3675,7 +3675,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3683,7 +3683,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3691,7 +3691,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3721,7 +3721,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3729,7 +3729,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3737,7 +3737,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3745,7 +3745,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3753,7 +3753,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3761,7 +3761,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3769,7 +3769,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3777,7 +3777,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3785,7 +3785,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3793,7 +3793,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3801,7 +3801,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3809,7 +3809,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3839,7 +3839,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3847,7 +3847,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3855,7 +3855,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3863,7 +3863,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3871,7 +3871,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3879,7 +3879,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3887,7 +3887,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3895,7 +3895,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3903,7 +3903,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3911,7 +3911,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3919,7 +3919,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3927,7 +3927,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3957,7 +3957,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3965,7 +3965,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3973,7 +3973,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3981,7 +3981,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3989,7 +3989,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -3997,7 +3997,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4005,7 +4005,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4013,7 +4013,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4021,7 +4021,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4029,7 +4029,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4037,7 +4037,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4045,7 +4045,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -4067,7 +4067,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4075,7 +4075,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4083,7 +4083,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4091,7 +4091,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4099,7 +4099,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4107,7 +4107,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4115,7 +4115,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4123,7 +4123,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4131,7 +4131,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4139,7 +4139,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4147,7 +4147,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4155,7 +4155,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4163,7 +4163,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -4185,7 +4185,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4193,7 +4193,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4201,7 +4201,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4209,7 +4209,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4217,7 +4217,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4225,7 +4225,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4233,7 +4233,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4241,7 +4241,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4249,7 +4249,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4257,7 +4257,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4265,7 +4265,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4273,7 +4273,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4281,7 +4281,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -4303,7 +4303,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4311,7 +4311,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4319,7 +4319,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4327,7 +4327,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4335,7 +4335,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4343,7 +4343,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4351,7 +4351,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4359,7 +4359,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4367,7 +4367,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4375,7 +4375,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4383,7 +4383,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4391,7 +4391,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4399,7 +4399,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -4421,7 +4421,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4429,7 +4429,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4437,7 +4437,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4445,7 +4445,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4453,7 +4453,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4461,7 +4461,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4469,7 +4469,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4477,7 +4477,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4485,7 +4485,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4493,7 +4493,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4501,7 +4501,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4509,7 +4509,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4517,7 +4517,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -4539,7 +4539,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4547,7 +4547,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4555,7 +4555,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4563,7 +4563,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4571,7 +4571,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4579,7 +4579,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4587,7 +4587,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4595,7 +4595,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4603,7 +4603,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4611,7 +4611,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4619,7 +4619,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4627,7 +4627,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4635,7 +4635,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -4657,7 +4657,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4665,7 +4665,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4673,7 +4673,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4681,7 +4681,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4689,7 +4689,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4697,7 +4697,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4705,7 +4705,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4713,7 +4713,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4721,7 +4721,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4729,7 +4729,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4737,7 +4737,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4745,7 +4745,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4753,7 +4753,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>